<commit_message>
Finaly gesture set selected. Closes #50
</commit_message>
<xml_diff>
--- a/Gesture_elicitation/Gesture_table.xlsx
+++ b/Gesture_elicitation/Gesture_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ieva\Documents\Coding\IIB_Project\Gesture_elicitation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10576AAD-EC61-43FE-9EB2-8D8FD93BAC26}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03775402-4C82-43F1-A45C-EB3134996EF5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{0FD874E3-1E4C-49D7-8375-9B1B8A2BC18A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
   <si>
     <t>Undo</t>
   </si>
@@ -96,9 +96,6 @@
     <t>New gesture no</t>
   </si>
   <si>
-    <t>Criteria</t>
-  </si>
-  <si>
     <t>Weight</t>
   </si>
   <si>
@@ -241,6 +238,18 @@
   </si>
   <si>
     <t>False positives rate</t>
+  </si>
+  <si>
+    <t>Qualities</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>COUPLED GESTURE SCORE BASED ON BEST GESTURE</t>
+  </si>
+  <si>
+    <t>UNDO + DELETE SCORE SUM BASED ON DELETE GESTURE</t>
   </si>
 </sst>
 </file>
@@ -248,7 +257,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -267,7 +276,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,6 +286,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -519,20 +534,31 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -849,16 +875,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BD36F5-6585-4231-8B92-87F12A5DCA57}">
   <dimension ref="A1:AQ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="B26" sqref="B26"/>
+      <selection pane="topRight" activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="18.796875" style="1" customWidth="1"/>
     <col min="2" max="7" width="13.59765625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.45">
@@ -908,7 +935,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="57" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:38" ht="85.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -954,18 +981,29 @@
       <c r="O2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="39" t="s">
+      <c r="P2" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q2" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="R2" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="R2" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="S2" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="T2" s="39" t="s">
+      <c r="S2" s="37" t="s">
         <v>65</v>
       </c>
+      <c r="T2" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="U2" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="X2" s="40"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
@@ -991,22 +1029,30 @@
       <c r="M3" s="9"/>
       <c r="N3" s="9"/>
       <c r="O3" s="10"/>
+      <c r="P3">
+        <v>0.9</v>
+      </c>
       <c r="Q3" s="32">
         <f>MAX(H22,N22,R22)</f>
-        <v>237</v>
+        <v>672.25</v>
       </c>
       <c r="R3" s="32">
         <f>LARGE((H22,N22,R22), 2)</f>
-        <v>226.19696969696969</v>
+        <v>664.33333333333326</v>
       </c>
       <c r="S3">
         <f>IF(Q3=$H$22,$B$1,IF(Q3=$N$22,$D$1,IF(Q3=$R$22,$F$1,0)))</f>
         <v>1</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="44">
         <f>IF(R3=$H$22,$B$1,IF(R3=$N$22,$D$1,IF(R3=$R$22,$F$1,0)))</f>
         <v>3</v>
       </c>
+      <c r="U3" s="41">
+        <f>P3*Q3+P4*R4</f>
+        <v>665.4589943330468</v>
+      </c>
+      <c r="V3" s="41"/>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
@@ -1023,22 +1069,30 @@
         <v>1</v>
       </c>
       <c r="O4" s="12"/>
+      <c r="P4">
+        <v>0.1</v>
+      </c>
       <c r="Q4" s="32">
         <f>MAX(L22,P22,T22)</f>
-        <v>222.9497320145615</v>
+        <v>621.16278579460266</v>
       </c>
       <c r="R4" s="32">
         <f>LARGE((L22,P22,T22), 2)</f>
-        <v>212.11986123415568</v>
-      </c>
-      <c r="S4">
+        <v>604.3399433304678</v>
+      </c>
+      <c r="S4" s="44">
         <f>IF(Q4=$L$22,$C$1,IF(Q4=$P$22,$E$1,IF(Q4=$T$22,$G$1,0)))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T4">
         <f>IF(R4=$L$22,$C$1,IF(R4=$P$22,$E$1,IF(R4=$T$22,$G$1,0)))</f>
-        <v>4</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="U4" s="41">
+        <f>P3*R3+P4*Q4</f>
+        <v>660.01627857946028</v>
+      </c>
+      <c r="V4" s="41"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
@@ -1055,22 +1109,30 @@
         <v>1</v>
       </c>
       <c r="O5" s="12"/>
+      <c r="P5">
+        <v>0.5</v>
+      </c>
       <c r="Q5" s="32">
         <f>MAX(V22,AB22,AF22)</f>
-        <v>217.29820810747293</v>
+        <v>627.3213890759597</v>
       </c>
       <c r="R5" s="32">
         <f>LARGE((V22,AB22,AF22), 2)</f>
-        <v>200.71187230465992</v>
+        <v>588.56836344717453</v>
       </c>
       <c r="S5">
         <f>IF(Q5=$V$22,$H$1,IF(Q5=$AB$22,$J$1,IF(Q5=$AF$22,$L$1,0)))</f>
         <v>7</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="44">
         <f>IF(R5=$V$22,$H$1,IF(R5=$AB$22,$J$1,IF(R5=$AF$22,$L$1,0)))</f>
         <v>11</v>
       </c>
+      <c r="U5" s="41">
+        <f>P5*Q5+P6*R6</f>
+        <v>557.97577776341257</v>
+      </c>
+      <c r="V5" s="41"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
@@ -1087,15 +1149,18 @@
         <v>1</v>
       </c>
       <c r="O6" s="12"/>
+      <c r="P6">
+        <v>0.5</v>
+      </c>
       <c r="Q6" s="32">
         <f>MAX(Z22,AD22,AH22)</f>
-        <v>220.68612426741174</v>
+        <v>612.83344265367316</v>
       </c>
       <c r="R6" s="32">
         <f>LARGE((Z22,AD22,AH22), 2)</f>
-        <v>196.57791416791605</v>
-      </c>
-      <c r="S6">
+        <v>488.63016645086543</v>
+      </c>
+      <c r="S6" s="44">
         <f>IF(Q6=$Z$22,$I$1,IF(Q6=$AD$22,$K$1,IF(Q6=$AH$22,$M$1,0)))</f>
         <v>12</v>
       </c>
@@ -1103,6 +1168,11 @@
         <f>IF(R6=$Z$22,$I$1,IF(R6=$AD$22,$K$1,IF(R6=$AH$22,$M$1,0)))</f>
         <v>8</v>
       </c>
+      <c r="U6" s="42">
+        <f>P5*R5+P6*Q6</f>
+        <v>600.7009030504239</v>
+      </c>
+      <c r="V6" s="42"/>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
@@ -1132,13 +1202,13 @@
       </c>
       <c r="Q7" s="32">
         <f>MAX(J22,X22,AJ22,AL22)</f>
-        <v>233</v>
+        <v>665.25</v>
       </c>
       <c r="R7" s="32">
         <f>LARGE((J22,X22,AJ22,AL22), 2)</f>
-        <v>208.40613980591215</v>
-      </c>
-      <c r="S7">
+        <v>625.49200285106292</v>
+      </c>
+      <c r="S7" s="44">
         <f>IF(Q7=$J$22,$B$1,IF(Q7=$X$22,$H$1,IF(Q7=$AJ$22,$N$1,IF(Q7=$AL$22,$O$1, 0))))</f>
         <v>1</v>
       </c>
@@ -1146,189 +1216,197 @@
         <f>IF(R7=$J$22,$B$1,IF(R7=$X$22,$H$1,IF(R7=$AJ$22,$N$1,IF(R7=$AL$22,$O$1, 0))))</f>
         <v>14</v>
       </c>
+      <c r="W7" s="43">
+        <f>Q7+U4</f>
+        <v>1325.2662785794603</v>
+      </c>
+      <c r="X7" s="32">
+        <f>R7+U3</f>
+        <v>1290.9509971841098</v>
+      </c>
     </row>
     <row r="9" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G9" s="34" t="s">
+      <c r="G9" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="39"/>
+      <c r="I9" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="35"/>
-      <c r="I9" s="34" t="s">
+      <c r="J9" s="39"/>
+      <c r="K9" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="35"/>
-      <c r="K9" s="34" t="s">
+      <c r="L9" s="39"/>
+      <c r="M9" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="35"/>
-      <c r="M9" s="34" t="s">
+      <c r="N9" s="39"/>
+      <c r="O9" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="N9" s="35"/>
-      <c r="O9" s="34" t="s">
+      <c r="P9" s="39"/>
+      <c r="Q9" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="P9" s="35"/>
-      <c r="Q9" s="34" t="s">
+      <c r="R9" s="39"/>
+      <c r="S9" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="R9" s="35"/>
-      <c r="S9" s="34" t="s">
+      <c r="T9" s="39"/>
+      <c r="U9" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="T9" s="35"/>
-      <c r="U9" s="34" t="s">
+      <c r="V9" s="39"/>
+      <c r="W9" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="V9" s="35"/>
-      <c r="W9" s="34" t="s">
+      <c r="X9" s="39"/>
+      <c r="Y9" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="X9" s="35"/>
-      <c r="Y9" s="34" t="s">
+      <c r="Z9" s="39"/>
+      <c r="AA9" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="Z9" s="35"/>
-      <c r="AA9" s="34" t="s">
+      <c r="AB9" s="39"/>
+      <c r="AC9" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="AB9" s="35"/>
-      <c r="AC9" s="34" t="s">
+      <c r="AD9" s="39"/>
+      <c r="AE9" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="AD9" s="35"/>
-      <c r="AE9" s="34" t="s">
+      <c r="AF9" s="39"/>
+      <c r="AG9" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH9" s="39"/>
+      <c r="AI9" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="AF9" s="35"/>
-      <c r="AG9" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="AH9" s="35"/>
-      <c r="AI9" s="34" t="s">
+      <c r="AJ9" s="39"/>
+      <c r="AK9" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="AJ9" s="35"/>
-      <c r="AK9" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="AL9" s="35"/>
+      <c r="AL9" s="39"/>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A10" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="23" t="s">
-        <v>22</v>
-      </c>
       <c r="C10" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="E10" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" s="11" t="s">
+      <c r="H10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="19" t="s">
-        <v>35</v>
-      </c>
       <c r="I10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="19" t="s">
-        <v>35</v>
-      </c>
       <c r="K10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="L10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="L10" s="19" t="s">
-        <v>35</v>
-      </c>
       <c r="M10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="N10" s="19" t="s">
-        <v>35</v>
-      </c>
       <c r="O10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="P10" s="19" t="s">
-        <v>35</v>
-      </c>
       <c r="Q10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="R10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="R10" s="19" t="s">
-        <v>35</v>
-      </c>
       <c r="S10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="T10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="T10" s="19" t="s">
-        <v>35</v>
-      </c>
       <c r="U10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="V10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="V10" s="19" t="s">
-        <v>35</v>
-      </c>
       <c r="W10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="X10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="X10" s="19" t="s">
-        <v>35</v>
-      </c>
       <c r="Y10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="Z10" s="19" t="s">
-        <v>35</v>
-      </c>
       <c r="AA10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="AB10" s="19" t="s">
-        <v>35</v>
-      </c>
       <c r="AC10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="AD10" s="19" t="s">
-        <v>35</v>
-      </c>
       <c r="AE10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="AF10" s="19" t="s">
-        <v>35</v>
-      </c>
       <c r="AG10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="AH10" s="19" t="s">
-        <v>35</v>
-      </c>
       <c r="AI10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="AJ10" s="19" t="s">
-        <v>35</v>
-      </c>
       <c r="AK10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL10" s="19" t="s">
         <v>34</v>
-      </c>
-      <c r="AL10" s="19" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:38" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A11" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1">
         <v>2</v>
@@ -1470,7 +1548,7 @@
     </row>
     <row r="12" spans="1:38" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1">
         <v>3</v>
@@ -1612,7 +1690,7 @@
     </row>
     <row r="13" spans="1:38" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A13" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1">
         <v>3</v>
@@ -1752,7 +1830,7 @@
     </row>
     <row r="14" spans="1:38" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A14" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="11">
         <v>5</v>
@@ -1894,7 +1972,7 @@
     </row>
     <row r="15" spans="1:38" ht="57" x14ac:dyDescent="0.45">
       <c r="A15" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="11">
         <v>1</v>
@@ -2040,10 +2118,10 @@
     </row>
     <row r="16" spans="1:38" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="11">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
@@ -2053,127 +2131,127 @@
       </c>
       <c r="E16" s="21">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="G16" s="26">
         <v>5</v>
       </c>
       <c r="H16" s="27">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="I16" s="31">
         <v>5</v>
       </c>
       <c r="J16" s="27">
         <f t="shared" ref="J16" si="62">I16*$B16</f>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="K16" s="26">
         <v>5</v>
       </c>
       <c r="L16" s="27">
         <f t="shared" ref="L16" si="63">K16*$B16</f>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="M16" s="26">
         <v>4.5</v>
       </c>
       <c r="N16" s="27">
         <f t="shared" ref="N16" si="64">M16*$B16</f>
-        <v>22.5</v>
+        <v>45</v>
       </c>
       <c r="O16" s="26">
         <v>4.5</v>
       </c>
       <c r="P16" s="27">
         <f t="shared" ref="P16" si="65">O16*$B16</f>
-        <v>22.5</v>
+        <v>45</v>
       </c>
       <c r="Q16" s="26">
         <v>4</v>
       </c>
       <c r="R16" s="27">
         <f t="shared" ref="R16" si="66">Q16*$B16</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="S16" s="26">
         <v>4</v>
       </c>
       <c r="T16" s="27">
         <f t="shared" ref="T16" si="67">S16*$B16</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="U16" s="26">
         <v>4.5</v>
       </c>
       <c r="V16" s="27">
         <f t="shared" ref="V16" si="68">U16*$B16</f>
-        <v>22.5</v>
+        <v>45</v>
       </c>
       <c r="W16" s="26">
         <v>4.5</v>
       </c>
       <c r="X16" s="27">
         <f t="shared" ref="X16" si="69">W16*$B16</f>
-        <v>22.5</v>
+        <v>45</v>
       </c>
       <c r="Y16" s="26">
         <v>4.5</v>
       </c>
       <c r="Z16" s="27">
         <f t="shared" ref="Z16" si="70">Y16*$B16</f>
-        <v>22.5</v>
+        <v>45</v>
       </c>
       <c r="AA16" s="26">
         <v>3</v>
       </c>
       <c r="AB16" s="27">
         <f t="shared" ref="AB16" si="71">AA16*$B16</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="AC16" s="26">
         <v>3</v>
       </c>
       <c r="AD16" s="27">
         <f t="shared" ref="AD16" si="72">AC16*$B16</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="AE16" s="26">
         <v>5</v>
       </c>
       <c r="AF16" s="27">
         <f t="shared" ref="AF16" si="73">AE16*$B16</f>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="AG16" s="26">
         <v>5</v>
       </c>
       <c r="AH16" s="27">
         <f t="shared" ref="AH16" si="74">AG16*$B16</f>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="AI16" s="26">
         <v>2</v>
       </c>
       <c r="AJ16" s="27">
         <f t="shared" ref="AJ16" si="75">AI16*$B16</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="AK16" s="26">
         <v>4.5</v>
       </c>
       <c r="AL16" s="27">
         <f t="shared" ref="AL16" si="76">AK16*$B16</f>
-        <v>22.5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" s="11">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
@@ -2183,7 +2261,7 @@
       </c>
       <c r="E17" s="21">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G17" s="26">
         <f>-(G$26-$C$28)/($C$28-$B$28)*5</f>
@@ -2191,7 +2269,7 @@
       </c>
       <c r="H17" s="27">
         <f t="shared" si="1"/>
-        <v>23.75</v>
+        <v>0</v>
       </c>
       <c r="I17" s="26">
         <f>-(I$26-$C$28)/($C$28-$B$28)*5</f>
@@ -2199,7 +2277,7 @@
       </c>
       <c r="J17" s="27">
         <f>I17*$B17</f>
-        <v>23.75</v>
+        <v>0</v>
       </c>
       <c r="K17" s="26">
         <f>-(K$26-$C$28)/($C$28-$B$28)*5</f>
@@ -2207,7 +2285,7 @@
       </c>
       <c r="L17" s="27">
         <f>K17*$B17</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="M17" s="26">
         <f>-(M$26-$C$28)/($C$28-$B$28)*5</f>
@@ -2215,7 +2293,7 @@
       </c>
       <c r="N17" s="27">
         <f>M17*$B17</f>
-        <v>13.863636363636365</v>
+        <v>0</v>
       </c>
       <c r="O17" s="26">
         <f>-(O$26-$C$28)/($C$28-$B$28)*5</f>
@@ -2223,7 +2301,7 @@
       </c>
       <c r="P17" s="27">
         <f>O17*$B17</f>
-        <v>11.704545454545453</v>
+        <v>0</v>
       </c>
       <c r="Q17" s="26">
         <f>-(Q$26-$C$28)/($C$28-$B$28)*5</f>
@@ -2231,7 +2309,7 @@
       </c>
       <c r="R17" s="27">
         <f>Q17*$B17</f>
-        <v>18.295454545454547</v>
+        <v>0</v>
       </c>
       <c r="S17" s="26">
         <f>-(S$26-$C$28)/($C$28-$B$28)*5</f>
@@ -2239,7 +2317,7 @@
       </c>
       <c r="T17" s="27">
         <f>S17*$B17</f>
-        <v>12.045454545454541</v>
+        <v>0</v>
       </c>
       <c r="U17" s="26">
         <f>-(U$26-$C$28)/($C$28-$B$28)*5</f>
@@ -2247,7 +2325,7 @@
       </c>
       <c r="V17" s="27">
         <f>U17*$B17</f>
-        <v>14.545454545454547</v>
+        <v>0</v>
       </c>
       <c r="W17" s="26">
         <f>-(W$26-$C$28)/($C$28-$B$28)*5</f>
@@ -2255,7 +2333,7 @@
       </c>
       <c r="X17" s="27">
         <f>W17*$B17</f>
-        <v>14.545454545454547</v>
+        <v>0</v>
       </c>
       <c r="Y17" s="26">
         <f>-(Y$26-$C$28)/($C$28-$B$28)*5</f>
@@ -2263,7 +2341,7 @@
       </c>
       <c r="Z17" s="27">
         <f>Y17*$B17</f>
-        <v>24.431818181818183</v>
+        <v>0</v>
       </c>
       <c r="AA17" s="26">
         <f>-(AA$26-$C$28)/($C$28-$B$28)*5</f>
@@ -2271,7 +2349,7 @@
       </c>
       <c r="AB17" s="27">
         <f>AA17*$B17</f>
-        <v>2.1590909090909074</v>
+        <v>0</v>
       </c>
       <c r="AC17" s="26">
         <f>-(AC$26-$C$28)/($C$28-$B$28)*5</f>
@@ -2287,7 +2365,7 @@
       </c>
       <c r="AF17" s="27">
         <f>AE17*$B17</f>
-        <v>10.454545454545453</v>
+        <v>0</v>
       </c>
       <c r="AG17" s="26">
         <f>-(AG$26-$C$28)/($C$28-$B$28)*5</f>
@@ -2295,7 +2373,7 @@
       </c>
       <c r="AH17" s="27">
         <f>AG17*$B17</f>
-        <v>15.909090909090908</v>
+        <v>0</v>
       </c>
       <c r="AI17" s="26">
         <f>-(AI$26-$C$28)/($C$28-$B$28)*5</f>
@@ -2303,7 +2381,7 @@
       </c>
       <c r="AJ17" s="27">
         <f>AI17*$B17</f>
-        <v>9.4318181818181834</v>
+        <v>0</v>
       </c>
       <c r="AK17" s="26">
         <f>-(AK$26-$C$28)/($C$28-$B$28)*5</f>
@@ -2311,15 +2389,15 @@
       </c>
       <c r="AL17" s="27">
         <f>AK17*$B17</f>
-        <v>12.613636363636363</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:43" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" s="11">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
@@ -2329,7 +2407,7 @@
       </c>
       <c r="E18" s="21">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="G18" s="26">
         <f>6/20*5</f>
@@ -2337,7 +2415,7 @@
       </c>
       <c r="H18" s="27">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="I18" s="31">
         <f>4/20*5</f>
@@ -2345,7 +2423,7 @@
       </c>
       <c r="J18" s="27">
         <f t="shared" ref="J18" si="77">I18*$B18</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="K18" s="26">
         <f>5/20*5</f>
@@ -2353,7 +2431,7 @@
       </c>
       <c r="L18" s="27">
         <f t="shared" ref="L18" si="78">K18*$B18</f>
-        <v>7.5</v>
+        <v>15</v>
       </c>
       <c r="M18" s="26">
         <f>3/20*5</f>
@@ -2361,7 +2439,7 @@
       </c>
       <c r="N18" s="27">
         <f t="shared" ref="N18" si="79">M18*$B18</f>
-        <v>4.5</v>
+        <v>9</v>
       </c>
       <c r="O18" s="26">
         <f>4/20*5</f>
@@ -2369,7 +2447,7 @@
       </c>
       <c r="P18" s="27">
         <f t="shared" ref="P18:P19" si="80">O18*$B18</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="Q18" s="26">
         <f>1/20*5</f>
@@ -2377,7 +2455,7 @@
       </c>
       <c r="R18" s="27">
         <f t="shared" ref="R18" si="81">Q18*$B18</f>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="S18" s="26">
         <f>3/20*5</f>
@@ -2385,7 +2463,7 @@
       </c>
       <c r="T18" s="27">
         <f t="shared" ref="T18" si="82">S18*$B18</f>
-        <v>4.5</v>
+        <v>9</v>
       </c>
       <c r="U18" s="26">
         <f>12/20*5</f>
@@ -2393,7 +2471,7 @@
       </c>
       <c r="V18" s="27">
         <f t="shared" ref="V18" si="83">U18*$B18</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="W18" s="26">
         <f>3/20*5</f>
@@ -2401,7 +2479,7 @@
       </c>
       <c r="X18" s="27">
         <f t="shared" ref="X18" si="84">W18*$B18</f>
-        <v>4.5</v>
+        <v>9</v>
       </c>
       <c r="Y18" s="26">
         <f>11/20*5</f>
@@ -2409,7 +2487,7 @@
       </c>
       <c r="Z18" s="27">
         <f t="shared" ref="Z18" si="85">Y18*$B18</f>
-        <v>16.5</v>
+        <v>33</v>
       </c>
       <c r="AA18" s="26">
         <f>1/20*5</f>
@@ -2417,7 +2495,7 @@
       </c>
       <c r="AB18" s="27">
         <f t="shared" ref="AB18" si="86">AA18*$B18</f>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="AC18" s="26">
         <f>1/20*5</f>
@@ -2425,7 +2503,7 @@
       </c>
       <c r="AD18" s="27">
         <f t="shared" ref="AD18" si="87">AC18*$B18</f>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="AE18" s="26">
         <f>3/20*5</f>
@@ -2433,7 +2511,7 @@
       </c>
       <c r="AF18" s="27">
         <f t="shared" ref="AF18" si="88">AE18*$B18</f>
-        <v>4.5</v>
+        <v>9</v>
       </c>
       <c r="AG18" s="26">
         <f>1/20*5</f>
@@ -2441,7 +2519,7 @@
       </c>
       <c r="AH18" s="27">
         <f t="shared" ref="AH18" si="89">AG18*$B18</f>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="AI18" s="26">
         <f>3/20*5</f>
@@ -2449,7 +2527,7 @@
       </c>
       <c r="AJ18" s="27">
         <f t="shared" ref="AJ18" si="90">AI18*$B18</f>
-        <v>4.5</v>
+        <v>9</v>
       </c>
       <c r="AK18" s="26">
         <f>3/20*5</f>
@@ -2457,15 +2535,15 @@
       </c>
       <c r="AL18" s="27">
         <f t="shared" ref="AL18" si="91">AK18*$B18</f>
-        <v>4.5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A19" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" s="11">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1">
         <v>0</v>
@@ -2475,7 +2553,7 @@
       </c>
       <c r="E19" s="21">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>150</v>
       </c>
       <c r="G19" s="26">
         <f>(G31-$E$31)/($D$31-$E$31)*5</f>
@@ -2483,7 +2561,7 @@
       </c>
       <c r="H19" s="27">
         <f t="shared" ref="H19:J19" si="92">G19*$B19</f>
-        <v>35</v>
+        <v>150</v>
       </c>
       <c r="I19" s="26">
         <f>(I31-$E$31)/($D$31-$E$31)*5</f>
@@ -2491,7 +2569,7 @@
       </c>
       <c r="J19" s="27">
         <f t="shared" si="92"/>
-        <v>35</v>
+        <v>150</v>
       </c>
       <c r="K19" s="26">
         <f>(K31-$E$31)/($D$31-$E$31)*5</f>
@@ -2499,7 +2577,7 @@
       </c>
       <c r="L19" s="27">
         <f t="shared" ref="L19" si="93">K19*$B19</f>
-        <v>33.793103448275858</v>
+        <v>144.82758620689654</v>
       </c>
       <c r="M19" s="26">
         <f>(M31-$E$31)/($D$31-$E$31)*5</f>
@@ -2507,7 +2585,7 @@
       </c>
       <c r="N19" s="27">
         <f t="shared" ref="N19" si="94">M19*$B19</f>
-        <v>35</v>
+        <v>150</v>
       </c>
       <c r="O19" s="26">
         <f>(O31-$E$31)/($D$31-$E$31)*5</f>
@@ -2515,7 +2593,7 @@
       </c>
       <c r="P19" s="27">
         <f t="shared" si="80"/>
-        <v>31.379310344827584</v>
+        <v>134.48275862068965</v>
       </c>
       <c r="Q19" s="26">
         <f>(Q31-$E$31)/($D$31-$E$31)*5</f>
@@ -2523,7 +2601,7 @@
       </c>
       <c r="R19" s="27">
         <f t="shared" ref="R19" si="95">Q19*$B19</f>
-        <v>27.758620689655174</v>
+        <v>118.96551724137932</v>
       </c>
       <c r="S19" s="26">
         <f>(S31-$E$31)/($D$31-$E$31)*5</f>
@@ -2539,7 +2617,7 @@
       </c>
       <c r="V19" s="27">
         <f t="shared" ref="V19" si="97">U19*$B19</f>
-        <v>32.586206896551722</v>
+        <v>139.65517241379308</v>
       </c>
       <c r="W19" s="26">
         <f>(W31-$E$31)/($D$31-$E$31)*5</f>
@@ -2547,7 +2625,7 @@
       </c>
       <c r="X19" s="27">
         <f t="shared" ref="X19" si="98">W19*$B19</f>
-        <v>32.586206896551722</v>
+        <v>139.65517241379308</v>
       </c>
       <c r="Y19" s="26">
         <f>(Y31-$E$31)/($D$31-$E$31)*5</f>
@@ -2555,7 +2633,7 @@
       </c>
       <c r="Z19" s="27">
         <f t="shared" ref="Z19" si="99">Y19*$B19</f>
-        <v>27.758620689655174</v>
+        <v>118.96551724137932</v>
       </c>
       <c r="AA19" s="26">
         <f>(AA31-$E$31)/($D$31-$E$31)*5</f>
@@ -2563,7 +2641,7 @@
       </c>
       <c r="AB19" s="27">
         <f t="shared" ref="AB19" si="100">AA19*$B19</f>
-        <v>21.724137931034484</v>
+        <v>93.103448275862064</v>
       </c>
       <c r="AC19" s="26">
         <f>(AC31-$E$31)/($D$31-$E$31)*5</f>
@@ -2571,7 +2649,7 @@
       </c>
       <c r="AD19" s="27">
         <f t="shared" ref="AD19" si="101">AC19*$B19</f>
-        <v>14.482758620689657</v>
+        <v>62.068965517241381</v>
       </c>
       <c r="AE19" s="26">
         <f>(AE31-$E$31)/($D$31-$E$31)*5</f>
@@ -2579,7 +2657,7 @@
       </c>
       <c r="AF19" s="27">
         <f t="shared" ref="AF19" si="102">AE19*$B19</f>
-        <v>30.172413793103445</v>
+        <v>129.31034482758619</v>
       </c>
       <c r="AG19" s="26">
         <f>(AG31-$E$31)/($D$31-$E$31)*5</f>
@@ -2587,7 +2665,7 @@
       </c>
       <c r="AH19" s="27">
         <f t="shared" ref="AH19" si="103">AG19*$B19</f>
-        <v>30.172413793103445</v>
+        <v>129.31034482758619</v>
       </c>
       <c r="AI19" s="26">
         <f>(AI31-$E$31)/($D$31-$E$31)*5</f>
@@ -2595,7 +2673,7 @@
       </c>
       <c r="AJ19" s="27">
         <f t="shared" ref="AJ19" si="104">AI19*$B19</f>
-        <v>26.551724137931036</v>
+        <v>113.79310344827586</v>
       </c>
       <c r="AK19" s="26">
         <f>(AK31-$E$31)/($D$31-$E$31)*5</f>
@@ -2603,15 +2681,15 @@
       </c>
       <c r="AL19" s="27">
         <f t="shared" ref="AL19" si="105">AK19*$B19</f>
-        <v>33.793103448275858</v>
+        <v>144.82758620689654</v>
       </c>
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="11">
         <v>30</v>
-      </c>
-      <c r="B20" s="11">
-        <v>8</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
@@ -2621,7 +2699,7 @@
       </c>
       <c r="E20" s="21">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="G20" s="26">
         <f>(G32-$E$32)/($D$32-$E$32)*5</f>
@@ -2629,7 +2707,7 @@
       </c>
       <c r="H20" s="27">
         <f t="shared" ref="H20:J20" si="106">G20*$B20</f>
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="I20" s="26">
         <f>(I32-$E$32)/($D$32-$E$32)*5</f>
@@ -2637,7 +2715,7 @@
       </c>
       <c r="J20" s="27">
         <f t="shared" si="106"/>
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="K20" s="26">
         <f>(K32-$E$32)/($D$32-$E$32)*5</f>
@@ -2645,7 +2723,7 @@
       </c>
       <c r="L20" s="27">
         <f t="shared" ref="L20" si="107">K20*$B20</f>
-        <v>22.856628566285664</v>
+        <v>85.712357123571238</v>
       </c>
       <c r="M20" s="26">
         <f>(M32-$E$32)/($D$32-$E$32)*5</f>
@@ -2653,7 +2731,7 @@
       </c>
       <c r="N20" s="27">
         <f t="shared" ref="N20" si="108">M20*$B20</f>
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="O20" s="26">
         <f>(O32-$E$32)/($D$32-$E$32)*5</f>
@@ -2661,7 +2739,7 @@
       </c>
       <c r="P20" s="27">
         <f t="shared" ref="P20" si="109">O20*$B20</f>
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="Q20" s="26">
         <f>(Q32-$E$32)/($D$32-$E$32)*5</f>
@@ -2669,7 +2747,7 @@
       </c>
       <c r="R20" s="27">
         <f t="shared" ref="R20" si="110">Q20*$B20</f>
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="S20" s="26">
         <f>(S32-$E$32)/($D$32-$E$32)*5</f>
@@ -2677,7 +2755,7 @@
       </c>
       <c r="T20" s="27">
         <f t="shared" ref="T20" si="111">S20*$B20</f>
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="U20" s="26">
         <f>(U32-$E$32)/($D$32-$E$32)*5</f>
@@ -2685,7 +2763,7 @@
       </c>
       <c r="V20" s="27">
         <f t="shared" ref="V20" si="112">U20*$B20</f>
-        <v>27.99987999879999</v>
+        <v>104.99954999549996</v>
       </c>
       <c r="W20" s="26">
         <f>(W32-$E$32)/($D$32-$E$32)*5</f>
@@ -2693,7 +2771,7 @@
       </c>
       <c r="X20" s="27">
         <f t="shared" ref="X20" si="113">W20*$B20</f>
-        <v>27.99987999879999</v>
+        <v>104.99954999549996</v>
       </c>
       <c r="Y20" s="26">
         <f>(Y32-$E$32)/($D$32-$E$32)*5</f>
@@ -2709,7 +2787,7 @@
       </c>
       <c r="AB20" s="27">
         <f t="shared" ref="AB20" si="115">AA20*$B20</f>
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="AC20" s="26">
         <f>(AC32-$E$32)/($D$32-$E$32)*5</f>
@@ -2717,7 +2795,7 @@
       </c>
       <c r="AD20" s="27">
         <f t="shared" ref="AD20" si="116">AC20*$B20</f>
-        <v>1.9512195121951281</v>
+        <v>7.3170731707317307</v>
       </c>
       <c r="AE20" s="26">
         <f>(AE32-$E$32)/($D$32-$E$32)*5</f>
@@ -2725,7 +2803,7 @@
       </c>
       <c r="AF20" s="27">
         <f t="shared" ref="AF20" si="117">AE20*$B20</f>
-        <v>30.399903999039996</v>
+        <v>113.99963999639998</v>
       </c>
       <c r="AG20" s="26">
         <f>(AG32-$E$32)/($D$32-$E$32)*5</f>
@@ -2733,7 +2811,7 @@
       </c>
       <c r="AH20" s="27">
         <f t="shared" ref="AH20" si="118">AG20*$B20</f>
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="AI20" s="26">
         <f>(AI32-$E$32)/($D$32-$E$32)*5</f>
@@ -2741,7 +2819,7 @@
       </c>
       <c r="AJ20" s="27">
         <f t="shared" ref="AJ20" si="119">AI20*$B20</f>
-        <v>4.9992499924999283</v>
+        <v>18.747187471874732</v>
       </c>
       <c r="AK20" s="26">
         <f>(AK32-$E$32)/($D$32-$E$32)*5</f>
@@ -2749,15 +2827,15 @@
       </c>
       <c r="AL20" s="27">
         <f t="shared" ref="AL20" si="120">AK20*$B20</f>
-        <v>33.332733327333266</v>
+        <v>124.99774997749975</v>
       </c>
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A21" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21" s="13">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C21" s="14">
         <v>0</v>
@@ -2767,7 +2845,7 @@
       </c>
       <c r="E21" s="22">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="G21" s="28">
         <f>-(G$33-$C$33)/($C$33-$B$33)*5</f>
@@ -2775,7 +2853,7 @@
       </c>
       <c r="H21" s="29">
         <f t="shared" ref="H21:J21" si="121">G21*$B21</f>
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="I21" s="28">
         <f>-(I$33-$C$33)/($C$33-$B$33)*5</f>
@@ -2783,7 +2861,7 @@
       </c>
       <c r="J21" s="29">
         <f t="shared" si="121"/>
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="K21" s="28">
         <f>-(K$33-$C$33)/($C$33-$B$33)*5</f>
@@ -2791,7 +2869,7 @@
       </c>
       <c r="L21" s="29">
         <f t="shared" ref="L21" si="122">K21*$B21</f>
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="M21" s="28">
         <f>-(M$33-$C$33)/($C$33-$B$33)*5</f>
@@ -2799,7 +2877,7 @@
       </c>
       <c r="N21" s="29">
         <f t="shared" ref="N21" si="123">M21*$B21</f>
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="O21" s="28">
         <f>-(O$33-$C$33)/($C$33-$B$33)*5</f>
@@ -2807,7 +2885,7 @@
       </c>
       <c r="P21" s="29">
         <f t="shared" ref="P21" si="124">O21*$B21</f>
-        <v>44.786005434782609</v>
+        <v>223.93002717391303</v>
       </c>
       <c r="Q21" s="28">
         <f>-(Q$33-$C$33)/($C$33-$B$33)*5</f>
@@ -2815,7 +2893,7 @@
       </c>
       <c r="R21" s="29">
         <f t="shared" ref="R21" si="125">Q21*$B21</f>
-        <v>39.656929347826093</v>
+        <v>198.28464673913047</v>
       </c>
       <c r="S21" s="28">
         <f>-(S$33-$C$33)/($C$33-$B$33)*5</f>
@@ -2831,7 +2909,7 @@
       </c>
       <c r="V21" s="29">
         <f t="shared" ref="V21" si="127">U21*$B21</f>
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="W21" s="28">
         <f>-(W$33-$C$33)/($C$33-$B$33)*5</f>
@@ -2839,7 +2917,7 @@
       </c>
       <c r="X21" s="29">
         <f t="shared" ref="X21" si="128">W21*$B21</f>
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="Y21" s="28">
         <f>-(Y$33-$C$33)/($C$33-$B$33)*5</f>
@@ -2847,7 +2925,7 @@
       </c>
       <c r="Z21" s="29">
         <f t="shared" ref="Z21" si="129">Y21*$B21</f>
-        <v>46.569293478260867</v>
+        <v>232.84646739130434</v>
       </c>
       <c r="AA21" s="28">
         <f>-(AA$33-$C$33)/($C$33-$B$33)*5</f>
@@ -2855,7 +2933,7 @@
       </c>
       <c r="AB21" s="29">
         <f t="shared" ref="AB21" si="130">AA21*$B21</f>
-        <v>30.859374999999996</v>
+        <v>154.29687499999997</v>
       </c>
       <c r="AC21" s="28">
         <f>-(AC$33-$C$33)/($C$33-$B$33)*5</f>
@@ -2863,7 +2941,7 @@
       </c>
       <c r="AD21" s="29">
         <f t="shared" ref="AD21" si="131">AC21*$B21</f>
-        <v>42.917798913043477</v>
+        <v>214.58899456521738</v>
       </c>
       <c r="AE21" s="28">
         <f>-(AE$33-$C$33)/($C$33-$B$33)*5</f>
@@ -2871,7 +2949,7 @@
       </c>
       <c r="AF21" s="29">
         <f t="shared" ref="AF21" si="132">AE21*$B21</f>
-        <v>46.518342391304344</v>
+        <v>232.59171195652172</v>
       </c>
       <c r="AG21" s="28">
         <f>-(AG$33-$C$33)/($C$33-$B$33)*5</f>
@@ -2879,7 +2957,7 @@
       </c>
       <c r="AH21" s="29">
         <f t="shared" ref="AH21" si="133">AG21*$B21</f>
-        <v>43.104619565217391</v>
+        <v>215.52309782608697</v>
       </c>
       <c r="AI21" s="28">
         <f>-(AI$33-$C$33)/($C$33-$B$33)*5</f>
@@ -2887,7 +2965,7 @@
       </c>
       <c r="AJ21" s="29">
         <f t="shared" ref="AJ21" si="134">AI21*$B21</f>
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="AK21" s="28">
         <f>-(AK$33-$C$33)/($C$33-$B$33)*5</f>
@@ -2895,87 +2973,87 @@
       </c>
       <c r="AL21" s="29">
         <f t="shared" ref="AL21" si="135">AK21*$B21</f>
-        <v>50</v>
+        <v>250</v>
       </c>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.45">
       <c r="E22" s="1">
         <f>SUM(E11:E21)</f>
-        <v>275</v>
+        <v>730</v>
       </c>
       <c r="H22" s="32">
         <f>SUM(H11:H21)</f>
-        <v>237</v>
+        <v>672.25</v>
       </c>
       <c r="J22" s="32">
         <f>SUM(J11:J21)</f>
-        <v>233</v>
+        <v>665.25</v>
       </c>
       <c r="L22" s="32">
         <f>SUM(L11:L21)</f>
-        <v>222.9497320145615</v>
+        <v>604.3399433304678</v>
       </c>
       <c r="N22" s="32">
         <f>SUM(N11:N21)</f>
-        <v>226.19696969696969</v>
+        <v>664.33333333333326</v>
       </c>
       <c r="P22" s="32">
         <f>SUM(P11:P21)</f>
-        <v>212.11986123415568</v>
+        <v>621.16278579460266</v>
       </c>
       <c r="R22" s="32">
         <f>SUM(R11:R21)</f>
-        <v>196.21100458293583</v>
+        <v>559.2501639805098</v>
       </c>
       <c r="T22" s="32">
         <f>SUM(T11:T21)</f>
-        <v>135.21212121212119</v>
+        <v>257.66666666666663</v>
       </c>
       <c r="V22" s="32">
         <f>SUM(V11:V21)</f>
-        <v>217.29820810747293</v>
+        <v>627.3213890759597</v>
       </c>
       <c r="X22" s="32">
         <f>SUM(X11:X21)</f>
-        <v>201.13154144080627</v>
+        <v>597.65472240929307</v>
       </c>
       <c r="Z22" s="32">
         <f>SUM(Z11:Z21)</f>
-        <v>196.57791416791605</v>
+        <v>488.63016645086543</v>
       </c>
       <c r="AB22" s="32">
         <f>SUM(AB11:AB21)</f>
-        <v>143.24260384012538</v>
+        <v>462.40032327586209</v>
       </c>
       <c r="AD22" s="32">
         <f>SUM(AD11:AD21)</f>
-        <v>107.85177704592826</v>
+        <v>348.97503325319047</v>
       </c>
       <c r="AF22" s="32">
         <f>SUM(AF11:AF21)</f>
-        <v>200.71187230465992</v>
+        <v>588.56836344717453</v>
       </c>
       <c r="AH22" s="32">
         <f>SUM(AH11:AH21)</f>
-        <v>220.68612426741174</v>
+        <v>612.83344265367316</v>
       </c>
       <c r="AJ22" s="32">
         <f>SUM(AJ11:AJ21)</f>
-        <v>151.81612564558247</v>
+        <v>457.87362425348391</v>
       </c>
       <c r="AL22" s="32">
         <f>SUM(AL11:AL21)</f>
-        <v>208.40613980591215</v>
+        <v>625.49200285106292</v>
       </c>
       <c r="AN22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AO22" s="32">
         <f>MAX(G22:AL22)</f>
-        <v>237</v>
+        <v>672.25</v>
       </c>
       <c r="AP22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AQ22">
         <f>MATCH(AO22,G22:AL22,0)</f>
@@ -2984,7 +3062,7 @@
     </row>
     <row r="26" spans="1:43" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A26" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B26" s="11">
         <v>-0.1</v>
@@ -3114,19 +3192,19 @@
     </row>
     <row r="27" spans="1:43" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="D27" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.45">
@@ -3155,384 +3233,384 @@
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37">
+        <v>57</v>
+      </c>
+      <c r="B31" s="35"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35">
         <f>MAX(G31,I31,K31,M31,O31,Q31,S31,U31,W31,Y31,AA31,AC31,AE31,AG31,AI31,AK31)</f>
         <v>1</v>
       </c>
-      <c r="E31" s="37">
+      <c r="E31" s="35">
         <f>MIN(G31,I31,K31,M31,O31,Q31,S31,U31,W31,Y31,AA31,AC31,AE31,AG31,AI31,AK31)</f>
         <v>0.97099999999999997</v>
       </c>
-      <c r="F31" s="37"/>
-      <c r="G31" s="36">
-        <v>1</v>
-      </c>
-      <c r="H31" s="38">
+      <c r="F31" s="35"/>
+      <c r="G31" s="34">
+        <v>1</v>
+      </c>
+      <c r="H31" s="36">
         <f>G31*$B19</f>
-        <v>7</v>
-      </c>
-      <c r="I31" s="36">
-        <v>1</v>
-      </c>
-      <c r="J31" s="38">
+        <v>30</v>
+      </c>
+      <c r="I31" s="34">
+        <v>1</v>
+      </c>
+      <c r="J31" s="36">
         <f>I31*$B19</f>
-        <v>7</v>
-      </c>
-      <c r="K31" s="36">
+        <v>30</v>
+      </c>
+      <c r="K31" s="34">
         <v>0.999</v>
       </c>
-      <c r="L31" s="38">
+      <c r="L31" s="36">
         <f>K31*$B19</f>
-        <v>6.9930000000000003</v>
-      </c>
-      <c r="M31" s="36">
-        <v>1</v>
-      </c>
-      <c r="N31" s="38">
+        <v>29.97</v>
+      </c>
+      <c r="M31" s="34">
+        <v>1</v>
+      </c>
+      <c r="N31" s="36">
         <f>M31*$B19</f>
-        <v>7</v>
-      </c>
-      <c r="O31" s="36">
+        <v>30</v>
+      </c>
+      <c r="O31" s="34">
         <v>0.997</v>
       </c>
-      <c r="P31" s="38">
+      <c r="P31" s="36">
         <f>O31*$B19</f>
-        <v>6.9790000000000001</v>
-      </c>
-      <c r="Q31" s="36">
+        <v>29.91</v>
+      </c>
+      <c r="Q31" s="34">
         <v>0.99399999999999999</v>
       </c>
-      <c r="R31" s="38">
+      <c r="R31" s="36">
         <f>Q31*$B19</f>
-        <v>6.9580000000000002</v>
-      </c>
-      <c r="S31" s="36">
+        <v>29.82</v>
+      </c>
+      <c r="S31" s="34">
         <v>0.97099999999999997</v>
       </c>
-      <c r="T31" s="38">
+      <c r="T31" s="36">
         <f>S31*$B19</f>
-        <v>6.7969999999999997</v>
-      </c>
-      <c r="U31" s="36">
+        <v>29.13</v>
+      </c>
+      <c r="U31" s="34">
         <v>0.998</v>
       </c>
-      <c r="V31" s="38">
+      <c r="V31" s="36">
         <f>U31*$B19</f>
-        <v>6.9859999999999998</v>
-      </c>
-      <c r="W31" s="36">
+        <v>29.94</v>
+      </c>
+      <c r="W31" s="34">
         <v>0.998</v>
       </c>
-      <c r="X31" s="38">
+      <c r="X31" s="36">
         <f>W31*$B19</f>
-        <v>6.9859999999999998</v>
-      </c>
-      <c r="Y31" s="36">
+        <v>29.94</v>
+      </c>
+      <c r="Y31" s="34">
         <v>0.99399999999999999</v>
       </c>
-      <c r="Z31" s="38">
+      <c r="Z31" s="36">
         <f>Y31*$B19</f>
-        <v>6.9580000000000002</v>
-      </c>
-      <c r="AA31" s="36">
+        <v>29.82</v>
+      </c>
+      <c r="AA31" s="34">
         <v>0.98899999999999999</v>
       </c>
-      <c r="AB31" s="38">
+      <c r="AB31" s="36">
         <f>AA31*$B19</f>
-        <v>6.923</v>
-      </c>
-      <c r="AC31" s="36">
+        <v>29.669999999999998</v>
+      </c>
+      <c r="AC31" s="34">
         <v>0.98299999999999998</v>
       </c>
-      <c r="AD31" s="38">
+      <c r="AD31" s="36">
         <f>AC31*$B19</f>
-        <v>6.8810000000000002</v>
-      </c>
-      <c r="AE31" s="36">
+        <v>29.49</v>
+      </c>
+      <c r="AE31" s="34">
         <v>0.996</v>
       </c>
-      <c r="AF31" s="38">
+      <c r="AF31" s="36">
         <f>AE31*$B19</f>
-        <v>6.9719999999999995</v>
-      </c>
-      <c r="AG31" s="36">
+        <v>29.88</v>
+      </c>
+      <c r="AG31" s="34">
         <v>0.996</v>
       </c>
-      <c r="AH31" s="38">
+      <c r="AH31" s="36">
         <f>AG31*$B19</f>
-        <v>6.9719999999999995</v>
-      </c>
-      <c r="AI31" s="36">
+        <v>29.88</v>
+      </c>
+      <c r="AI31" s="34">
         <v>0.99299999999999999</v>
       </c>
-      <c r="AJ31" s="38">
+      <c r="AJ31" s="36">
         <f>AI31*$B19</f>
-        <v>6.9509999999999996</v>
-      </c>
-      <c r="AK31" s="36">
+        <v>29.79</v>
+      </c>
+      <c r="AK31" s="34">
         <v>0.999</v>
       </c>
-      <c r="AL31" s="38">
+      <c r="AL31" s="36">
         <f>AK31*$B19</f>
-        <v>6.9930000000000003</v>
+        <v>29.97</v>
       </c>
     </row>
     <row r="32" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37">
+        <v>58</v>
+      </c>
+      <c r="B32" s="35"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35">
         <f>MAX(G32,I32,K32,M32,O32,Q32,S32,U32,W32,Y32,AA32,AC32,AE32,AG32,AI32,AK32)</f>
         <v>1</v>
       </c>
-      <c r="E32" s="37">
+      <c r="E32" s="35">
         <f>MIN(G32,I32,K32,M32,O32,Q32,S32,U32,W32,Y32,AA32,AC32,AE32,AG32,AI32,AK32)</f>
         <v>0.66666999999999998</v>
       </c>
-      <c r="F32" s="37"/>
-      <c r="G32" s="37">
-        <v>1</v>
-      </c>
-      <c r="H32" s="38">
+      <c r="F32" s="35"/>
+      <c r="G32" s="35">
+        <v>1</v>
+      </c>
+      <c r="H32" s="36">
         <f t="shared" ref="H32:J33" si="136">G32*$B20</f>
-        <v>8</v>
-      </c>
-      <c r="I32" s="37">
-        <v>1</v>
-      </c>
-      <c r="J32" s="38">
+        <v>30</v>
+      </c>
+      <c r="I32" s="35">
+        <v>1</v>
+      </c>
+      <c r="J32" s="36">
         <f t="shared" si="136"/>
-        <v>8</v>
-      </c>
-      <c r="K32" s="36">
+        <v>30</v>
+      </c>
+      <c r="K32" s="34">
         <v>0.85714000000000001</v>
       </c>
-      <c r="L32" s="38">
+      <c r="L32" s="36">
         <f t="shared" ref="L32" si="137">K32*$B20</f>
-        <v>6.8571200000000001</v>
-      </c>
-      <c r="M32" s="36">
-        <v>1</v>
-      </c>
-      <c r="N32" s="38">
+        <v>25.714200000000002</v>
+      </c>
+      <c r="M32" s="34">
+        <v>1</v>
+      </c>
+      <c r="N32" s="36">
         <f t="shared" ref="N32" si="138">M32*$B20</f>
-        <v>8</v>
-      </c>
-      <c r="O32" s="36">
-        <v>1</v>
-      </c>
-      <c r="P32" s="38">
+        <v>30</v>
+      </c>
+      <c r="O32" s="34">
+        <v>1</v>
+      </c>
+      <c r="P32" s="36">
         <f t="shared" ref="P32" si="139">O32*$B20</f>
-        <v>8</v>
-      </c>
-      <c r="Q32" s="36">
-        <v>1</v>
-      </c>
-      <c r="R32" s="38">
+        <v>30</v>
+      </c>
+      <c r="Q32" s="34">
+        <v>1</v>
+      </c>
+      <c r="R32" s="36">
         <f t="shared" ref="R32" si="140">Q32*$B20</f>
-        <v>8</v>
-      </c>
-      <c r="S32" s="36">
-        <v>1</v>
-      </c>
-      <c r="T32" s="38">
+        <v>30</v>
+      </c>
+      <c r="S32" s="34">
+        <v>1</v>
+      </c>
+      <c r="T32" s="36">
         <f t="shared" ref="T32" si="141">S32*$B20</f>
-        <v>8</v>
-      </c>
-      <c r="U32" s="36">
+        <v>30</v>
+      </c>
+      <c r="U32" s="34">
         <v>0.9</v>
       </c>
-      <c r="V32" s="38">
+      <c r="V32" s="36">
         <f t="shared" ref="V32" si="142">U32*$B20</f>
-        <v>7.2</v>
-      </c>
-      <c r="W32" s="36">
+        <v>27</v>
+      </c>
+      <c r="W32" s="34">
         <v>0.9</v>
       </c>
-      <c r="X32" s="38">
+      <c r="X32" s="36">
         <f t="shared" ref="X32" si="143">W32*$B20</f>
-        <v>7.2</v>
-      </c>
-      <c r="Y32" s="36">
+        <v>27</v>
+      </c>
+      <c r="Y32" s="34">
         <v>0.66666999999999998</v>
       </c>
-      <c r="Z32" s="38">
+      <c r="Z32" s="36">
         <f t="shared" ref="Z32" si="144">Y32*$B20</f>
-        <v>5.3333599999999999</v>
-      </c>
-      <c r="AA32" s="36">
-        <v>1</v>
-      </c>
-      <c r="AB32" s="38">
+        <v>20.0001</v>
+      </c>
+      <c r="AA32" s="34">
+        <v>1</v>
+      </c>
+      <c r="AB32" s="36">
         <f t="shared" ref="AB32" si="145">AA32*$B20</f>
-        <v>8</v>
-      </c>
-      <c r="AC32" s="36">
+        <v>30</v>
+      </c>
+      <c r="AC32" s="34">
         <v>0.68293000000000004</v>
       </c>
-      <c r="AD32" s="38">
+      <c r="AD32" s="36">
         <f t="shared" ref="AD32" si="146">AC32*$B20</f>
-        <v>5.4634400000000003</v>
-      </c>
-      <c r="AE32" s="36">
+        <v>20.4879</v>
+      </c>
+      <c r="AE32" s="34">
         <v>0.92</v>
       </c>
-      <c r="AF32" s="38">
+      <c r="AF32" s="36">
         <f t="shared" ref="AF32" si="147">AE32*$B20</f>
-        <v>7.36</v>
-      </c>
-      <c r="AG32" s="36">
-        <v>1</v>
-      </c>
-      <c r="AH32" s="38">
+        <v>27.6</v>
+      </c>
+      <c r="AG32" s="34">
+        <v>1</v>
+      </c>
+      <c r="AH32" s="36">
         <f t="shared" ref="AH32" si="148">AG32*$B20</f>
-        <v>8</v>
-      </c>
-      <c r="AI32" s="36">
+        <v>30</v>
+      </c>
+      <c r="AI32" s="34">
         <v>0.70833000000000002</v>
       </c>
-      <c r="AJ32" s="38">
+      <c r="AJ32" s="36">
         <f t="shared" ref="AJ32" si="149">AI32*$B20</f>
-        <v>5.6666400000000001</v>
-      </c>
-      <c r="AK32" s="36">
+        <v>21.2499</v>
+      </c>
+      <c r="AK32" s="34">
         <v>0.94443999999999995</v>
       </c>
-      <c r="AL32" s="38">
+      <c r="AL32" s="36">
         <f t="shared" ref="AL32" si="150">AK32*$B20</f>
-        <v>7.5555199999999996</v>
+        <v>28.333199999999998</v>
       </c>
     </row>
     <row r="33" spans="1:38" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B33" s="37">
+        <v>59</v>
+      </c>
+      <c r="B33" s="35">
         <f>MIN(G33,I33,K33,M33,O33,Q33,S33,U33,W33,Y33,AA33,AC33,AE33,AG33,AI33,AK33)</f>
         <v>0</v>
       </c>
-      <c r="C33" s="37">
+      <c r="C33" s="35">
         <f>MAX(G33,I33,K33,M33,O33,Q33,S33,U33,W33,Y33,AA33,AC33,AE33,AG33,AI33,AK33)</f>
         <v>2.9440000000000001E-2</v>
       </c>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37">
-        <v>0</v>
-      </c>
-      <c r="H33" s="38">
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35">
+        <v>0</v>
+      </c>
+      <c r="H33" s="36">
         <f t="shared" si="136"/>
         <v>0</v>
       </c>
-      <c r="I33" s="37">
-        <v>0</v>
-      </c>
-      <c r="J33" s="38">
+      <c r="I33" s="35">
+        <v>0</v>
+      </c>
+      <c r="J33" s="36">
         <f t="shared" si="136"/>
         <v>0</v>
       </c>
-      <c r="K33" s="36">
-        <v>0</v>
-      </c>
-      <c r="L33" s="38">
+      <c r="K33" s="34">
+        <v>0</v>
+      </c>
+      <c r="L33" s="36">
         <f t="shared" ref="L33" si="151">K33*$B21</f>
         <v>0</v>
       </c>
-      <c r="M33" s="36">
-        <v>0</v>
-      </c>
-      <c r="N33" s="38">
+      <c r="M33" s="34">
+        <v>0</v>
+      </c>
+      <c r="N33" s="36">
         <f t="shared" ref="N33" si="152">M33*$B21</f>
         <v>0</v>
       </c>
-      <c r="O33" s="36">
+      <c r="O33" s="34">
         <v>3.0699999999999998E-3</v>
       </c>
-      <c r="P33" s="38">
+      <c r="P33" s="36">
         <f t="shared" ref="P33" si="153">O33*$B21</f>
-        <v>3.0699999999999998E-2</v>
-      </c>
-      <c r="Q33" s="36">
+        <v>0.1535</v>
+      </c>
+      <c r="Q33" s="34">
         <v>6.0899999999999999E-3</v>
       </c>
-      <c r="R33" s="38">
+      <c r="R33" s="36">
         <f t="shared" ref="R33" si="154">Q33*$B21</f>
-        <v>6.0899999999999996E-2</v>
-      </c>
-      <c r="S33" s="36">
+        <v>0.30449999999999999</v>
+      </c>
+      <c r="S33" s="34">
         <v>2.9440000000000001E-2</v>
       </c>
-      <c r="T33" s="38">
+      <c r="T33" s="36">
         <f t="shared" ref="T33" si="155">S33*$B21</f>
-        <v>0.2944</v>
-      </c>
-      <c r="U33" s="36">
-        <v>0</v>
-      </c>
-      <c r="V33" s="38">
+        <v>1.472</v>
+      </c>
+      <c r="U33" s="34">
+        <v>0</v>
+      </c>
+      <c r="V33" s="36">
         <f t="shared" ref="V33" si="156">U33*$B21</f>
         <v>0</v>
       </c>
-      <c r="W33" s="36">
-        <v>0</v>
-      </c>
-      <c r="X33" s="38">
+      <c r="W33" s="34">
+        <v>0</v>
+      </c>
+      <c r="X33" s="36">
         <f t="shared" ref="X33" si="157">W33*$B21</f>
         <v>0</v>
       </c>
-      <c r="Y33" s="36">
+      <c r="Y33" s="34">
         <v>2.0200000000000001E-3</v>
       </c>
-      <c r="Z33" s="38">
+      <c r="Z33" s="36">
         <f t="shared" ref="Z33" si="158">Y33*$B21</f>
-        <v>2.0200000000000003E-2</v>
-      </c>
-      <c r="AA33" s="36">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="AA33" s="34">
         <v>1.1270000000000001E-2</v>
       </c>
-      <c r="AB33" s="38">
+      <c r="AB33" s="36">
         <f t="shared" ref="AB33" si="159">AA33*$B21</f>
-        <v>0.11270000000000001</v>
-      </c>
-      <c r="AC33" s="36">
+        <v>0.5635</v>
+      </c>
+      <c r="AC33" s="34">
         <v>4.1700000000000001E-3</v>
       </c>
-      <c r="AD33" s="38">
+      <c r="AD33" s="36">
         <f t="shared" ref="AD33" si="160">AC33*$B21</f>
-        <v>4.1700000000000001E-2</v>
-      </c>
-      <c r="AE33" s="36">
+        <v>0.20850000000000002</v>
+      </c>
+      <c r="AE33" s="34">
         <v>2.0500000000000002E-3</v>
       </c>
-      <c r="AF33" s="38">
+      <c r="AF33" s="36">
         <f t="shared" ref="AF33" si="161">AE33*$B21</f>
-        <v>2.0500000000000001E-2</v>
-      </c>
-      <c r="AG33" s="36">
+        <v>0.10250000000000001</v>
+      </c>
+      <c r="AG33" s="34">
         <v>4.0600000000000002E-3</v>
       </c>
-      <c r="AH33" s="38">
+      <c r="AH33" s="36">
         <f t="shared" ref="AH33" si="162">AG33*$B21</f>
-        <v>4.0600000000000004E-2</v>
-      </c>
-      <c r="AI33" s="36">
-        <v>0</v>
-      </c>
-      <c r="AJ33" s="38">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="AI33" s="34">
+        <v>0</v>
+      </c>
+      <c r="AJ33" s="36">
         <f t="shared" ref="AJ33" si="163">AI33*$B21</f>
         <v>0</v>
       </c>
-      <c r="AK33" s="36">
-        <v>0</v>
-      </c>
-      <c r="AL33" s="38">
+      <c r="AK33" s="34">
+        <v>0</v>
+      </c>
+      <c r="AL33" s="36">
         <f t="shared" ref="AL33" si="164">AK33*$B21</f>
         <v>0</v>
       </c>
@@ -3550,7 +3628,13 @@
       <c r="E35" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="22">
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="U6:V6"/>
     <mergeCell ref="Q9:R9"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="I9:J9"/>

</xml_diff>